<commit_message>
Change code to read CourseraOnlineCourses.xlsx file
Added Coursera data
Added summation graph and code
</commit_message>
<xml_diff>
--- a/CourseraOnlineCourses.xlsx
+++ b/CourseraOnlineCourses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abbi_\PycharmProjects\sumLinkedInLearningHours\Online_Courses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8EC62EB-B3EC-48A7-843F-7DB62CADE85B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE655BB2-B646-4073-8A06-DBF99A98CC80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{A4470D73-8618-4FD2-B64A-974AA8E5C036}"/>
   </bookViews>
@@ -397,7 +397,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -543,10 +543,6 @@
       <c r="D7">
         <v>390</v>
       </c>
-      <c r="F7">
-        <f>SUM(F2:F6)</f>
-        <v>463</v>
-      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8">
@@ -555,14 +551,6 @@
       <c r="B8">
         <v>77</v>
       </c>
-      <c r="D8">
-        <f>SUM(D2:D7)</f>
-        <v>781</v>
-      </c>
-      <c r="F8">
-        <f>F7/60</f>
-        <v>7.7166666666666668</v>
-      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9">
@@ -570,10 +558,6 @@
       </c>
       <c r="B9">
         <v>64</v>
-      </c>
-      <c r="D9">
-        <f>D8/60</f>
-        <v>13.016666666666667</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update Coursera hours and graphs
</commit_message>
<xml_diff>
--- a/CourseraOnlineCourses.xlsx
+++ b/CourseraOnlineCourses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abbi_\PycharmProjects\sumLinkedInLearningHours\Online_Courses\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE655BB2-B646-4073-8A06-DBF99A98CC80}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1726F347-3DD7-48F7-9E0A-314C37FC06AB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5640" xr2:uid="{A4470D73-8618-4FD2-B64A-974AA8E5C036}"/>
   </bookViews>
@@ -25,24 +25,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>c_dsMathSkills_hours</t>
-  </si>
-  <si>
-    <t>c_dsMathSkills_minutes</t>
   </si>
   <si>
     <t>c_total_hours</t>
   </si>
   <si>
-    <t>c_total_minutes</t>
-  </si>
-  <si>
     <t>c_AWSml_hours</t>
   </si>
   <si>
-    <t>c_AWSml_minutes</t>
+    <t>c_CV_hours</t>
+  </si>
+  <si>
+    <t>c_matlab_hours</t>
   </si>
 </sst>
 </file>
@@ -394,194 +391,54 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8416788-4BCA-428E-A539-4F9A3505C9BB}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="12.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>0</v>
+        <f>SUM(B2:E2)</f>
+        <v>66</v>
       </c>
       <c r="B2">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D2">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>120</v>
-      </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3">
-        <v>120</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>86</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4">
-        <v>86</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>87</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>87</v>
-      </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>81</v>
-      </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6">
-        <v>81</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>390</v>
-      </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7">
-        <v>390</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>186</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>